<commit_message>
Fluint wait added in utility
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -59,25 +59,25 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
+    <t xml:space="preserve">Firefox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suite1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suite2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smoke</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suite1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Firefox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suite2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smoke</t>
   </si>
   <si>
     <t xml:space="preserve">Suite3</t>
@@ -570,17 +570,17 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,10 +637,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="E4" s="3" t="n">
         <f aca="false">IF(B4="Y",COUNTIF(Suite2!B1:B12,"Y"),0)</f>
@@ -649,13 +649,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>16</v>
@@ -929,10 +929,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,10 +1081,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,7 +1188,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>